<commit_message>
added _types.ts and refined design
</commit_message>
<xml_diff>
--- a/data/example-config.xlsx
+++ b/data/example-config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofnottm-my.sharepoint.com/personal/chris_greenhalgh_nottingham_ac_uk/Documents/Projects/Music VQ Elizabeth 2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmg/workspace/music-class-chat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{F0717421-E5A0-1044-BF50-E78E6639129E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EC0F7434-04B0-4540-960D-880C6FCC75D6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DEAB70F-D5AC-5B4B-8875-E02748A9C5EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1440" windowWidth="24640" windowHeight="14000" activeTab="5" xr2:uid="{E8A503D0-EC5A-E746-BAA9-7113C281CDDE}"/>
+    <workbookView xWindow="-27260" yWindow="460" windowWidth="24640" windowHeight="14000" activeTab="4" xr2:uid="{E8A503D0-EC5A-E746-BAA9-7113C281CDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="123">
   <si>
     <t>public</t>
   </si>
@@ -50,9 +50,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>guest</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -101,12 +98,6 @@
     <t>short title</t>
   </si>
   <si>
-    <t>allow guest without password</t>
-  </si>
-  <si>
-    <t>required by users</t>
-  </si>
-  <si>
     <t>list on site:</t>
   </si>
   <si>
@@ -372,6 +363,51 @@
   </si>
   <si>
     <t>Well done, you're ready to go</t>
+  </si>
+  <si>
+    <t>slug for URL</t>
+  </si>
+  <si>
+    <t>requireinitials</t>
+  </si>
+  <si>
+    <t>requirepin</t>
+  </si>
+  <si>
+    <t>allowselfenrol2</t>
+  </si>
+  <si>
+    <t>requireemail</t>
+  </si>
+  <si>
+    <t>allowguest</t>
+  </si>
+  <si>
+    <t>for/from each user</t>
+  </si>
+  <si>
+    <t>for user access</t>
+  </si>
+  <si>
+    <t>i.e. email link when created (not stored)</t>
+  </si>
+  <si>
+    <t>or admin only</t>
+  </si>
+  <si>
+    <t>allow guest without password or memory</t>
+  </si>
+  <si>
+    <t>for selfregistration</t>
+  </si>
+  <si>
+    <t>slug for URL (and sheet name)</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Part 2</t>
   </si>
 </sst>
 </file>
@@ -427,7 +463,13 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="70">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -646,120 +688,126 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3660917E-F28B-E24F-B8CB-7116A007FD03}" name="Table2" displayName="Table2" ref="A1:E2" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{48620DAF-4E3F-1246-A190-36A889772123}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{514523A6-8825-1B49-AEE9-54F98410AC30}" name="name" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{F44AEC02-CEDC-D746-BAC2-53003C435AB0}" name="description" dataDxfId="66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3660917E-F28B-E24F-B8CB-7116A007FD03}" name="Table2" displayName="Table2" ref="A1:J2" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{48620DAF-4E3F-1246-A190-36A889772123}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{514523A6-8825-1B49-AEE9-54F98410AC30}" name="name" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{F77A5C71-F88D-FD4C-A507-978DA6898272}" name="_id" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F44AEC02-CEDC-D746-BAC2-53003C435AB0}" name="description" dataDxfId="68"/>
     <tableColumn id="3" xr3:uid="{10FC9B76-E9F4-4440-BABE-1179F4F61988}" name="public"/>
-    <tableColumn id="4" xr3:uid="{DCAB4E55-5A0B-F943-BFC8-85D795B22B91}" name="guest"/>
-    <tableColumn id="5" xr3:uid="{E24660F6-4566-4640-8EB4-A473C9462D91}" name="password" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{896435D6-E0FB-A142-940E-1B5FDCBAC91D}" name="requireinitials"/>
+    <tableColumn id="9" xr3:uid="{A78EDCB8-F7B4-054E-9397-935777507A8A}" name="requirepin"/>
+    <tableColumn id="8" xr3:uid="{E73F6E95-5D72-7341-94B3-C28A2BAD8FA4}" name="requireemail"/>
+    <tableColumn id="7" xr3:uid="{95B16D5B-2EC2-1042-ADBB-7257078A6BD0}" name="allowselfenrol2"/>
+    <tableColumn id="4" xr3:uid="{DCAB4E55-5A0B-F943-BFC8-85D795B22B91}" name="allowguest"/>
+    <tableColumn id="5" xr3:uid="{E24660F6-4566-4640-8EB4-A473C9462D91}" name="password" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC33DAED-8B40-2544-B087-DDF69FF66ECC}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC33DAED-8B40-2544-B087-DDF69FF66ECC}" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0" dataDxfId="66">
   <autoFilter ref="A1:D10" xr:uid="{A0226A79-3B4F-CE40-8B64-1DAFAD80F509}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B1952672-FA76-8244-A817-C7FF5E7BBCC3}" name="_id" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{A4BABDC0-8353-104D-9897-1182219AA6E9}" name="icon" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{295BA006-D777-C94C-9A3B-CBCE6DFA30F7}" name="noicon" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{6DB67210-B9D7-984E-9299-85DD07F56828}" name="comment" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{B1952672-FA76-8244-A817-C7FF5E7BBCC3}" name="_id" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{A4BABDC0-8353-104D-9897-1182219AA6E9}" name="icon" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{295BA006-D777-C94C-9A3B-CBCE6DFA30F7}" name="noicon" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{6DB67210-B9D7-984E-9299-85DD07F56828}" name="comment" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{46CC7FC3-C398-E54A-8F0F-67C0FFA584F9}" name="Table6" displayName="Table6" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{E6246C16-1458-2446-86A3-56CB4DDF4212}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{14EACF44-C26D-C241-8D88-1DC9DB8FCF0D}" name="name" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{89511BC0-8A83-6245-BB1D-AA3BBE172266}" name="description" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{942A6288-00A2-5544-B50C-650370B9F125}" name="icon" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{2185EE55-A940-F946-A627-49D344ED51AB}" name="sortorder" dataDxfId="56"/>
-    <tableColumn id="5" xr3:uid="{D03B7F16-DD48-D044-9A94-387DF9E748D4}" name="ifall" dataDxfId="55"/>
-    <tableColumn id="6" xr3:uid="{ADE9A9F1-7512-7E41-924F-A2B8D11FB01C}" name="andnot" dataDxfId="54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{46CC7FC3-C398-E54A-8F0F-67C0FFA584F9}" name="Table6" displayName="Table6" ref="A1:G7" totalsRowShown="0">
+  <autoFilter ref="A1:G7" xr:uid="{E6246C16-1458-2446-86A3-56CB4DDF4212}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{14EACF44-C26D-C241-8D88-1DC9DB8FCF0D}" name="name" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{7246BEBC-13A8-EB46-90C3-1EA396465A79}" name="_id" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{89511BC0-8A83-6245-BB1D-AA3BBE172266}" name="description" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{942A6288-00A2-5544-B50C-650370B9F125}" name="icon" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{2185EE55-A940-F946-A627-49D344ED51AB}" name="sortorder" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{D03B7F16-DD48-D044-9A94-387DF9E748D4}" name="ifall" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{ADE9A9F1-7512-7E41-924F-A2B8D11FB01C}" name="andnot" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D5C0D842-BB95-3948-9E74-73C8655AA488}" name="Table8" displayName="Table8" ref="A1:Q22" totalsRowShown="0" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D5C0D842-BB95-3948-9E74-73C8655AA488}" name="Table8" displayName="Table8" ref="A1:Q22" totalsRowShown="0" dataDxfId="55">
   <autoFilter ref="A1:Q22" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{98209BBC-74B8-0C48-8788-C46719605874}" name="label" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{67E33C65-F324-5447-9B5E-CD7DEA820D5F}" name="ifall" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{96F4C912-DDCB-9343-ABC8-65914498E850}" name="andnot" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{3C49259E-D837-304B-AEF0-D0E2D9F1CFFF}" name="after" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{BD167AE1-ADDC-D34F-A91C-94AA598E624A}" name="waitfor" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{BE72769F-64DC-AE49-A803-DDC74261D522}" name="ornext" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{3D9CBAD6-6312-FF40-B0BA-D5463A6E6774}" name="message" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{1BE9E1EF-0CDE-E84E-993D-DE2429DEF690}" name="type" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{2F612D43-F908-6E4E-8D31-EC869F33F6E9}" name="url" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{8A769766-7E92-F748-BAB6-502136570385}" name="title" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{84647AA4-DC4E-6042-938A-8DD06D6FEE16}" name="description" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{4C0CC8EC-5DF9-EF40-A394-04179633987D}" name="section" dataDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{3EC412FF-9AC2-D14B-8F4E-F9DBD3BA4519}" name="sortorder" dataDxfId="40"/>
-    <tableColumn id="14" xr3:uid="{3519660E-5EAF-8D4D-8894-76FFA8BA0976}" name="hidden" dataDxfId="39"/>
-    <tableColumn id="15" xr3:uid="{7E07B26D-13A3-0444-AC8A-C296741EFB75}" name="rewards" dataDxfId="38"/>
-    <tableColumn id="16" xr3:uid="{817F2933-35C9-4C45-AA59-74EB42A0D73E}" name="reset" dataDxfId="37"/>
-    <tableColumn id="17" xr3:uid="{8B62FD90-4BF1-0D40-843E-3CA898042B40}" name="jumpto" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{98209BBC-74B8-0C48-8788-C46719605874}" name="label" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{67E33C65-F324-5447-9B5E-CD7DEA820D5F}" name="ifall" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{96F4C912-DDCB-9343-ABC8-65914498E850}" name="andnot" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{3C49259E-D837-304B-AEF0-D0E2D9F1CFFF}" name="after" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{BD167AE1-ADDC-D34F-A91C-94AA598E624A}" name="waitfor" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{BE72769F-64DC-AE49-A803-DDC74261D522}" name="ornext" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{3D9CBAD6-6312-FF40-B0BA-D5463A6E6774}" name="message" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{1BE9E1EF-0CDE-E84E-993D-DE2429DEF690}" name="type" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{2F612D43-F908-6E4E-8D31-EC869F33F6E9}" name="url" dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{8A769766-7E92-F748-BAB6-502136570385}" name="title" dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{84647AA4-DC4E-6042-938A-8DD06D6FEE16}" name="description" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{4C0CC8EC-5DF9-EF40-A394-04179633987D}" name="section" dataDxfId="43"/>
+    <tableColumn id="13" xr3:uid="{3EC412FF-9AC2-D14B-8F4E-F9DBD3BA4519}" name="sortorder" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{3519660E-5EAF-8D4D-8894-76FFA8BA0976}" name="hidden" dataDxfId="41"/>
+    <tableColumn id="15" xr3:uid="{7E07B26D-13A3-0444-AC8A-C296741EFB75}" name="rewards" dataDxfId="40"/>
+    <tableColumn id="16" xr3:uid="{817F2933-35C9-4C45-AA59-74EB42A0D73E}" name="reset" dataDxfId="39"/>
+    <tableColumn id="17" xr3:uid="{8B62FD90-4BF1-0D40-843E-3CA898042B40}" name="jumpto" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0B2A40C4-7877-474D-AF59-BB042BA0FC6D}" name="Table810" displayName="Table810" ref="A1:Q22" totalsRowShown="0" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0B2A40C4-7877-474D-AF59-BB042BA0FC6D}" name="Table810" displayName="Table810" ref="A1:Q22" totalsRowShown="0" dataDxfId="37">
   <autoFilter ref="A1:Q22" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{2B440253-680B-2247-B853-0979AE53EDD8}" name="label" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{1A484451-0875-C749-B2F5-7E5897DE5603}" name="ifall" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{104A9865-E04C-3147-8C1B-4E4F83F04636}" name="andnot" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{56115264-3302-2542-81BE-FF30A56B9C54}" name="after" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{A294F377-14F0-D94F-88EB-910B6B34D824}" name="waitfor" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{936A0470-DEF3-8247-A24D-428C870F35E0}" name="ornext" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{7BFBE5EC-8CDB-0644-9EC0-AAEF93718DFB}" name="message" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{0FEACC26-B678-8944-A462-ADB539D13642}" name="type" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{0D022D26-1092-FF45-A0D8-CC149074B846}" name="url" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{19BDB18B-88B7-9E48-A2FE-488E75BA84C2}" name="title" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{AB56076E-698E-D841-8B1A-622FF0DB045F}" name="description" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{48ABAADE-729A-7843-BA82-8F26C2542086}" name="section" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{D7B394A7-C4A0-1A4A-A1E7-AD17CB0589A8}" name="sortorder" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{1CADD3D5-7424-074A-B60C-904978AE200C}" name="hidden" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{4ADA220A-13B5-B048-9C88-1C06EBC9D22C}" name="rewards" dataDxfId="20"/>
-    <tableColumn id="16" xr3:uid="{5CA885B2-6C6B-8E43-9687-61B995EBBD98}" name="reset" dataDxfId="19"/>
-    <tableColumn id="17" xr3:uid="{2E3DD60E-38B7-FD44-AC56-FEB0F8BFFDB9}" name="jumpto" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{2B440253-680B-2247-B853-0979AE53EDD8}" name="label" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{1A484451-0875-C749-B2F5-7E5897DE5603}" name="ifall" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{104A9865-E04C-3147-8C1B-4E4F83F04636}" name="andnot" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{56115264-3302-2542-81BE-FF30A56B9C54}" name="after" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{A294F377-14F0-D94F-88EB-910B6B34D824}" name="waitfor" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{936A0470-DEF3-8247-A24D-428C870F35E0}" name="ornext" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{7BFBE5EC-8CDB-0644-9EC0-AAEF93718DFB}" name="message" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{0FEACC26-B678-8944-A462-ADB539D13642}" name="type" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{0D022D26-1092-FF45-A0D8-CC149074B846}" name="url" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{19BDB18B-88B7-9E48-A2FE-488E75BA84C2}" name="title" dataDxfId="27"/>
+    <tableColumn id="11" xr3:uid="{AB56076E-698E-D841-8B1A-622FF0DB045F}" name="description" dataDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{48ABAADE-729A-7843-BA82-8F26C2542086}" name="section" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{D7B394A7-C4A0-1A4A-A1E7-AD17CB0589A8}" name="sortorder" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{1CADD3D5-7424-074A-B60C-904978AE200C}" name="hidden" dataDxfId="23"/>
+    <tableColumn id="15" xr3:uid="{4ADA220A-13B5-B048-9C88-1C06EBC9D22C}" name="rewards" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{5CA885B2-6C6B-8E43-9687-61B995EBBD98}" name="reset" dataDxfId="21"/>
+    <tableColumn id="17" xr3:uid="{2E3DD60E-38B7-FD44-AC56-FEB0F8BFFDB9}" name="jumpto" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97C05CA8-913E-2240-AF00-ACE7860C25D2}" name="Table81011" displayName="Table81011" ref="A1:Q22" totalsRowShown="0" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{97C05CA8-913E-2240-AF00-ACE7860C25D2}" name="Table81011" displayName="Table81011" ref="A1:Q22" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="A1:Q22" xr:uid="{669026F6-523A-EF49-B01A-F3286CFBC418}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{014A9763-B087-2B4B-93D7-75431119447F}" name="label" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{A4F9E4B9-5020-3C48-8665-3E8315A0B800}" name="ifall" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{1C7E0588-7912-3944-B0E6-43A61005CDCE}" name="andnot" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{8989FA64-7FB9-C247-B9BF-20B65C4D95A2}" name="after" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{62F0408F-976B-8D45-A227-44C809DD9B35}" name="waitfor" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{A72246FC-95B5-7746-85BD-39E49FE857EF}" name="ornext" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{1CB87543-7FEE-464F-B329-C58A29625D94}" name="message" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{05DA1C54-AE4B-D24D-9360-B6E0EE37D865}" name="type" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{A498DA27-4109-B34B-A2AE-B2B47AA9376F}" name="url" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{A44C8647-66DB-574E-974A-54DC42A0394F}" name="title" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{116F4944-FAF5-1B4A-94BC-EF69D91BB31F}" name="description" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{63D38E18-E427-0E4F-8896-96FBAEFE303D}" name="section" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{3E26E2C5-6A81-4A42-9801-75F4DCAE94DD}" name="sortorder" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{45B6A2D2-7510-174B-B316-E6B99B21CA61}" name="hidden" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{07A739DF-1EF3-C84D-A0AA-5AC780A62237}" name="rewards" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{1A794E51-2011-174A-94E7-B84BDA0472FE}" name="reset" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{BE08941E-FE4B-484F-9017-CAA09458CEFB}" name="jumpto" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{014A9763-B087-2B4B-93D7-75431119447F}" name="label" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{A4F9E4B9-5020-3C48-8665-3E8315A0B800}" name="ifall" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{1C7E0588-7912-3944-B0E6-43A61005CDCE}" name="andnot" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{8989FA64-7FB9-C247-B9BF-20B65C4D95A2}" name="after" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{62F0408F-976B-8D45-A227-44C809DD9B35}" name="waitfor" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{A72246FC-95B5-7746-85BD-39E49FE857EF}" name="ornext" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{1CB87543-7FEE-464F-B329-C58A29625D94}" name="message" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{05DA1C54-AE4B-D24D-9360-B6E0EE37D865}" name="type" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{A498DA27-4109-B34B-A2AE-B2B47AA9376F}" name="url" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{A44C8647-66DB-574E-974A-54DC42A0394F}" name="title" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{116F4944-FAF5-1B4A-94BC-EF69D91BB31F}" name="description" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{63D38E18-E427-0E4F-8896-96FBAEFE303D}" name="section" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{3E26E2C5-6A81-4A42-9801-75F4DCAE94DD}" name="sortorder" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{45B6A2D2-7510-174B-B316-E6B99B21CA61}" name="hidden" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{07A739DF-1EF3-C84D-A0AA-5AC780A62237}" name="rewards" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{1A794E51-2011-174A-94E7-B84BDA0472FE}" name="reset" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{BE08941E-FE4B-484F-9017-CAA09458CEFB}" name="jumpto" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1062,87 +1110,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD53B3AB-ED71-BA47-8C18-E2C026DCC1A5}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:E2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="24.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2" xr:uid="{D7A7EEC9-EFC5-1848-98FE-2FBE199149B0}">
-      <formula1>$C$6:$C$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 I2 E2:H2" xr:uid="{D7A7EEC9-EFC5-1848-98FE-2FBE199149B0}">
+      <formula1>$D$6:$D$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1156,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA4BC58-8D9E-8247-A221-EA67BCFA1E88}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A2:D10"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,80 +1262,80 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1273,18 +1366,18 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1297,146 +1390,166 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289E85D3-7FB2-A24E-9691-D911BF786AE9}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A2:F7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
         <v>17</v>
       </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1452,7 +1565,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1460,7 +1573,7 @@
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" customWidth="1"/>
-    <col min="7" max="7" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" customWidth="1"/>
     <col min="11" max="11" width="12.5" customWidth="1"/>
@@ -1470,55 +1583,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
       </c>
       <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
         <v>54</v>
       </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
         <v>57</v>
-      </c>
-      <c r="O1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -1529,7 +1642,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1548,29 +1661,29 @@
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -1583,29 +1696,31 @@
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -1618,29 +1733,29 @@
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1653,29 +1768,29 @@
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1688,29 +1803,29 @@
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="L7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1723,11 +1838,11 @@
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1737,7 +1852,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -2029,88 +2144,88 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="F25" t="s">
         <v>67</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>68</v>
       </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
         <v>69</v>
       </c>
-      <c r="F25" t="s">
+      <c r="J25" t="s">
         <v>70</v>
       </c>
-      <c r="G25" t="s">
+      <c r="L25" t="s">
         <v>71</v>
       </c>
-      <c r="H25" t="s">
+      <c r="N25" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" t="s">
         <v>72</v>
       </c>
-      <c r="J25" t="s">
+      <c r="P25" t="s">
         <v>73</v>
       </c>
-      <c r="L25" t="s">
+      <c r="Q25" t="s">
         <v>74</v>
-      </c>
-      <c r="N25" t="s">
-        <v>7</v>
-      </c>
-      <c r="O25" t="s">
-        <v>75</v>
-      </c>
-      <c r="P25" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2139,7 +2254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB17B971-6F00-E840-82DA-EE647268194B}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -2156,55 +2271,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
       </c>
       <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
         <v>54</v>
       </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
         <v>57</v>
-      </c>
-      <c r="O1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2215,7 +2330,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2225,7 +2340,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -2236,11 +2351,11 @@
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2250,10 +2365,10 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="Q3" s="1"/>
     </row>
@@ -2639,88 +2754,88 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="F25" t="s">
         <v>67</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>68</v>
       </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
         <v>69</v>
       </c>
-      <c r="F25" t="s">
+      <c r="J25" t="s">
         <v>70</v>
       </c>
-      <c r="G25" t="s">
+      <c r="L25" t="s">
         <v>71</v>
       </c>
-      <c r="H25" t="s">
+      <c r="N25" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" t="s">
         <v>72</v>
       </c>
-      <c r="J25" t="s">
+      <c r="P25" t="s">
         <v>73</v>
       </c>
-      <c r="L25" t="s">
+      <c r="Q25" t="s">
         <v>74</v>
-      </c>
-      <c r="N25" t="s">
-        <v>7</v>
-      </c>
-      <c r="O25" t="s">
-        <v>75</v>
-      </c>
-      <c r="P25" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2746,7 +2861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B819C41-D178-6849-96F5-6846425DFC81}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
@@ -2763,55 +2878,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
       </c>
       <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
         <v>54</v>
       </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
         <v>57</v>
-      </c>
-      <c r="O1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -2822,7 +2937,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2832,7 +2947,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -2843,11 +2958,11 @@
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2857,10 +2972,10 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="1"/>
     </row>
@@ -3246,88 +3361,88 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="F25" t="s">
         <v>67</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>68</v>
       </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
         <v>69</v>
       </c>
-      <c r="F25" t="s">
+      <c r="J25" t="s">
         <v>70</v>
       </c>
-      <c r="G25" t="s">
+      <c r="L25" t="s">
         <v>71</v>
       </c>
-      <c r="H25" t="s">
+      <c r="N25" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" t="s">
         <v>72</v>
       </c>
-      <c r="J25" t="s">
+      <c r="P25" t="s">
         <v>73</v>
       </c>
-      <c r="L25" t="s">
+      <c r="Q25" t="s">
         <v>74</v>
-      </c>
-      <c r="N25" t="s">
-        <v>7</v>
-      </c>
-      <c r="O25" t="s">
-        <v>75</v>
-      </c>
-      <c r="P25" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added _servertypes and first test view
</commit_message>
<xml_diff>
--- a/data/example-config.xlsx
+++ b/data/example-config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmg/workspace/music-class-chat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DEAB70F-D5AC-5B4B-8875-E02748A9C5EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87156D87-BD54-3743-BF21-E226B581A210}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27260" yWindow="460" windowWidth="24640" windowHeight="14000" activeTab="4" xr2:uid="{E8A503D0-EC5A-E746-BAA9-7113C281CDDE}"/>
+    <workbookView xWindow="-27260" yWindow="460" windowWidth="24640" windowHeight="14000" xr2:uid="{E8A503D0-EC5A-E746-BAA9-7113C281CDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="124">
   <si>
     <t>public</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>Part 2</t>
+  </si>
+  <si>
+    <t>Test 1</t>
   </si>
 </sst>
 </file>
@@ -692,7 +695,7 @@
   <autoFilter ref="A1:J2" xr:uid="{48620DAF-4E3F-1246-A190-36A889772123}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{514523A6-8825-1B49-AEE9-54F98410AC30}" name="name" dataDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{F77A5C71-F88D-FD4C-A507-978DA6898272}" name="_id" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F77A5C71-F88D-FD4C-A507-978DA6898272}" name="_id" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{F44AEC02-CEDC-D746-BAC2-53003C435AB0}" name="description" dataDxfId="68"/>
     <tableColumn id="3" xr3:uid="{10FC9B76-E9F4-4440-BABE-1179F4F61988}" name="public"/>
     <tableColumn id="10" xr3:uid="{896435D6-E0FB-A142-940E-1B5FDCBAC91D}" name="requireinitials"/>
@@ -724,7 +727,7 @@
   <autoFilter ref="A1:G7" xr:uid="{E6246C16-1458-2446-86A3-56CB4DDF4212}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{14EACF44-C26D-C241-8D88-1DC9DB8FCF0D}" name="name" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{7246BEBC-13A8-EB46-90C3-1EA396465A79}" name="_id" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{7246BEBC-13A8-EB46-90C3-1EA396465A79}" name="_id" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{89511BC0-8A83-6245-BB1D-AA3BBE172266}" name="description" dataDxfId="60"/>
     <tableColumn id="3" xr3:uid="{942A6288-00A2-5544-B50C-650370B9F125}" name="icon" dataDxfId="59"/>
     <tableColumn id="4" xr3:uid="{2185EE55-A940-F946-A627-49D344ED51AB}" name="sortorder" dataDxfId="58"/>
@@ -1112,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD53B3AB-ED71-BA47-8C18-E2C026DCC1A5}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,6 +1164,9 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1234,7 +1240,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 I2 E2:H2" xr:uid="{D7A7EEC9-EFC5-1848-98FE-2FBE199149B0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I2" xr:uid="{D7A7EEC9-EFC5-1848-98FE-2FBE199149B0}">
       <formula1>$D$6:$D$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -2254,7 +2260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB17B971-6F00-E840-82DA-EE647268194B}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bug fix import; add test icons; add user content
</commit_message>
<xml_diff>
--- a/data/example-config.xlsx
+++ b/data/example-config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmg/workspace/music-class-chat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1CA100-6B90-A341-9304-28A0876FAAC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E898DD3B-9452-E048-ACC6-A5B8B92AC1FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27260" yWindow="460" windowWidth="24640" windowHeight="14000" activeTab="1" xr2:uid="{E8A503D0-EC5A-E746-BAA9-7113C281CDDE}"/>
+    <workbookView xWindow="-27260" yWindow="460" windowWidth="24640" windowHeight="14000" activeTab="3" xr2:uid="{E8A503D0-EC5A-E746-BAA9-7113C281CDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -275,9 +275,6 @@
     <t>Here's an image</t>
   </si>
   <si>
-    <t>image.png</t>
-  </si>
-  <si>
     <t>An image</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>Here's an audio file</t>
   </si>
   <si>
-    <t>music.mp3</t>
-  </si>
-  <si>
     <t>Some audio</t>
   </si>
   <si>
@@ -405,6 +399,12 @@
   </si>
   <si>
     <t>allowselfenrol</t>
+  </si>
+  <si>
+    <t>http://www.cs.nott.ac.uk/~pszcmg/massive1/thumbnail/chi1.gif</t>
+  </si>
+  <si>
+    <t>https://music-mrl.nott.ac.uk/2/losing-her-voice/assets/habanera-short.mp3</t>
   </si>
 </sst>
 </file>
@@ -1135,22 +1135,22 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" t="s">
         <v>107</v>
-      </c>
-      <c r="G1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" t="s">
-        <v>109</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -1198,28 +1198,28 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="I5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA4BC58-8D9E-8247-A221-EA67BCFA1E88}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>36</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>33</v>
@@ -1537,7 +1537,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -1564,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE9F943-FBE9-CA48-8381-FDD6A6E3E5D1}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1670,20 +1670,20 @@
       <c r="H3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -1702,25 +1702,25 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -1733,29 +1733,29 @@
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1768,29 +1768,29 @@
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1807,25 +1807,25 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>59</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2242,10 +2242,12 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{C1EC6FD1-2229-7247-978D-380F8DA7BB62}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{341A34F9-A921-674E-9D19-B6BC061EA23E}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{010879BA-83D9-5146-AB91-341AD1189A89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2255,7 +2257,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>